<commit_message>
Bulk upload tester file header validate
</commit_message>
<xml_diff>
--- a/public/files/tester/Tester_Bulk_Upload_Excel_format.xlsx
+++ b/public/files/tester/Tester_Bulk_Upload_Excel_format.xlsx
@@ -50,7 +50,27 @@
     <t xml:space="preserve">Email*</t>
   </si>
   <si>
-    <t xml:space="preserve">Prefered Contact Method*</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Prefered Contact Method* </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Phone or Email)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Current Job Title*</t>
@@ -180,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,11 +213,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -280,11 +296,11 @@
   </sheetPr>
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
@@ -293,7 +309,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="34.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.43"/>
@@ -312,10 +328,10 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">

</xml_diff>

<commit_message>
Bulk upload tester file add upload option
</commit_message>
<xml_diff>
--- a/public/files/tester/Tester_Bulk_Upload_Excel_format.xlsx
+++ b/public/files/tester/Tester_Bulk_Upload_Excel_format.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t xml:space="preserve">Professional Registration No
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Professional Registration No*
 (if available)</t>
   </si>
   <si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Middle Name (3rd name)</t>
   </si>
   <si>
-    <t xml:space="preserve">Last Name (Surname)*</t>
+    <t xml:space="preserve">Last Name (Surname)</t>
   </si>
   <si>
     <t xml:space="preserve">Province*</t>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">Districts*</t>
   </si>
   <si>
-    <t xml:space="preserve">Type of HIV Test Modality/Point*</t>
+    <t xml:space="preserve">Type of HIV Test Modality/Point</t>
   </si>
   <si>
     <t xml:space="preserve">Phone*</t>
@@ -50,57 +50,34 @@
     <t xml:space="preserve">Email*</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Prefered Contact Method* </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FFC9211E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Phone or Email)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Current Job Title*</t>
+    <t xml:space="preserve">Prefered Contact Method (Phone or Email)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Job Title</t>
   </si>
   <si>
     <t xml:space="preserve">Facility Name*</t>
   </si>
   <si>
-    <t xml:space="preserve">Time Worked As Tester*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Site In charge Name*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing Site In charge Phone*</t>
+    <t xml:space="preserve">Time Worked As Tester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Site In charge Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Site In charge Phone</t>
   </si>
   <si>
     <t xml:space="preserve">Testing Site In charge Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Facility In charge Name*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facility In charge Phone*</t>
+    <t xml:space="preserve">Facility In charge Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility In charge Phone</t>
   </si>
   <si>
     <t xml:space="preserve">Facility In charge Email</t>
@@ -138,6 +115,7 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
+      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -145,7 +123,7 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FFC9211E"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -153,9 +131,9 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
-      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,7 +178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,8 +191,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -294,59 +276,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="34.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="34.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="17.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -355,7 +336,7 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -370,20 +351,17 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>